<commit_message>
Calculate optimization bounds for each NPP considered
</commit_message>
<xml_diff>
--- a/use_cases/IES_Feb23/data/HERON_data.xlsx
+++ b/use_cases/IES_Feb23/data/HERON_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11009"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrm/FORCE/use_cases/IES_Feb23/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36AA2432-313B-6342-A376-C4BA4C209AC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{160E53F7-2C21-874C-BC96-45BE68DCA324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20200" activeTab="5" xr2:uid="{3CE7F202-39F9-48AF-B0C7-575379157397}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17800" windowHeight="22400" activeTab="4" xr2:uid="{3CE7F202-39F9-48AF-B0C7-575379157397}"/>
   </bookViews>
   <sheets>
     <sheet name="MACRS" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="FT" sheetId="11" r:id="rId4"/>
     <sheet name="Boundaries" sheetId="10" r:id="rId5"/>
     <sheet name="Capacity_Market" sheetId="3" r:id="rId6"/>
+    <sheet name="NPP_capacities" sheetId="12" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="193">
   <si>
     <t>Source</t>
   </si>
@@ -469,6 +470,156 @@
   </si>
   <si>
     <t>100 kg initially stored, upper bound ~ 4h of storage for max capacity of FT</t>
+  </si>
+  <si>
+    <t>Plant</t>
+  </si>
+  <si>
+    <t>Market</t>
+  </si>
+  <si>
+    <t>Reactor type</t>
+  </si>
+  <si>
+    <t># Units</t>
+  </si>
+  <si>
+    <t>Capacity (MWth)</t>
+  </si>
+  <si>
+    <t>Capacity (MWe)</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>State corporate income tax rate (%)</t>
+  </si>
+  <si>
+    <t>Braidwood</t>
+  </si>
+  <si>
+    <t>PJM</t>
+  </si>
+  <si>
+    <t>PWR</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Braidwood_Nuclear_Generating_Station</t>
+  </si>
+  <si>
+    <t>Illinois</t>
+  </si>
+  <si>
+    <t>Davis-Besse</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Davis–Besse_Nuclear_Power_Station</t>
+  </si>
+  <si>
+    <t>Ohio</t>
+  </si>
+  <si>
+    <t>South Texas Project</t>
+  </si>
+  <si>
+    <t>ERCOT</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/South_Texas_Nuclear_Generating_Station</t>
+  </si>
+  <si>
+    <t>Texas</t>
+  </si>
+  <si>
+    <t>Diablo Canyon</t>
+  </si>
+  <si>
+    <t>CAISO</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Diablo_Canyon_Power_Plant</t>
+  </si>
+  <si>
+    <t>California</t>
+  </si>
+  <si>
+    <t>Prairie Island</t>
+  </si>
+  <si>
+    <t>MISO</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Prairie_Island_Nuclear_Power_Plant</t>
+  </si>
+  <si>
+    <t>Minnesota</t>
+  </si>
+  <si>
+    <t>Cooper Nuclear Station</t>
+  </si>
+  <si>
+    <t>SPP</t>
+  </si>
+  <si>
+    <t>BWR</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Cooper_Nuclear_Station</t>
+  </si>
+  <si>
+    <t>Nebraska</t>
+  </si>
+  <si>
+    <t>Palo Verde</t>
+  </si>
+  <si>
+    <t>Southwest, Arizona</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Palo_Verde_Nuclear_Generating_Station</t>
+  </si>
+  <si>
+    <t>Arizona</t>
+  </si>
+  <si>
+    <t>1194/1160</t>
+  </si>
+  <si>
+    <t>1138/1118</t>
+  </si>
+  <si>
+    <t>522/519</t>
+  </si>
+  <si>
+    <t>1311/1314/1312</t>
+  </si>
+  <si>
+    <t>Effective tax rate</t>
+  </si>
+  <si>
+    <t>Federal corporate tax rate</t>
+  </si>
+  <si>
+    <t>Cooper</t>
+  </si>
+  <si>
+    <t>HTSE Lower (MWe)</t>
+  </si>
+  <si>
+    <t>HTSE Upper (MWe)</t>
+  </si>
+  <si>
+    <t>FT Lower (kg-H2)</t>
+  </si>
+  <si>
+    <t>FT Upper (kg-H2)</t>
+  </si>
+  <si>
+    <t>H2 storage Lower (kg-H2)</t>
+  </si>
+  <si>
+    <t>H2 storage Upper (kg-h2)</t>
   </si>
 </sst>
 </file>
@@ -478,7 +629,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -512,6 +663,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -625,12 +783,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -657,12 +816,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2965,40 +3128,124 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9241F20-95C4-42A2-B03A-23B9DD4DBFA3}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="47.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.33203125" customWidth="1"/>
+    <col min="11" max="11" width="13.6640625" customWidth="1"/>
+    <col min="12" max="12" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>96</v>
       </c>
       <c r="B1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E1" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="G1" t="s">
+        <v>187</v>
+      </c>
+      <c r="H1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I1" t="s">
+        <v>189</v>
+      </c>
+      <c r="J1" t="s">
+        <v>190</v>
+      </c>
+      <c r="K1" t="s">
+        <v>191</v>
+      </c>
+      <c r="L1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>87</v>
       </c>
       <c r="B2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E2" t="s">
+        <v>151</v>
+      </c>
+      <c r="F2" s="23">
+        <v>1194</v>
+      </c>
+      <c r="G2">
+        <f>-F2+15</f>
+        <v>-1179</v>
+      </c>
+      <c r="H2">
+        <v>-400</v>
+      </c>
+      <c r="I2">
+        <f>G2*25.13</f>
+        <v>-29628.27</v>
+      </c>
+      <c r="J2">
+        <f>H2*25.13</f>
+        <v>-10052</v>
+      </c>
+      <c r="K2">
+        <v>500</v>
+      </c>
+      <c r="L2">
+        <f>ABS(I2)*4</f>
+        <v>118513.08</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
+        <v>156</v>
+      </c>
+      <c r="F3" s="23">
+        <v>894</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G8" si="0">-F3+15</f>
+        <v>-879</v>
+      </c>
+      <c r="H3">
+        <v>-400</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I8" si="1">G3*25.13</f>
+        <v>-22089.27</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J8" si="2">H3*25.13</f>
+        <v>-10052</v>
+      </c>
+      <c r="K3">
+        <v>500</v>
+      </c>
+      <c r="L3">
+        <f t="shared" ref="L3:L8" si="3">ABS(I3)*4</f>
+        <v>88357.08</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>84</v>
       </c>
@@ -3008,8 +3255,36 @@
       <c r="C4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E4" t="s">
+        <v>159</v>
+      </c>
+      <c r="F4" s="23">
+        <v>1280</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>-1265</v>
+      </c>
+      <c r="H4">
+        <v>-400</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="1"/>
+        <v>-31789.449999999997</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="2"/>
+        <v>-10052</v>
+      </c>
+      <c r="K4">
+        <v>500</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="3"/>
+        <v>127157.79999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>139</v>
       </c>
@@ -3019,8 +3294,36 @@
       <c r="C5" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E5" t="s">
+        <v>163</v>
+      </c>
+      <c r="F5" s="23">
+        <v>1138</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>-1123</v>
+      </c>
+      <c r="H5">
+        <v>-400</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="1"/>
+        <v>-28220.989999999998</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="2"/>
+        <v>-10052</v>
+      </c>
+      <c r="K5">
+        <v>500</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="3"/>
+        <v>112883.95999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>105</v>
       </c>
@@ -3030,8 +3333,36 @@
       <c r="C6" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E6" t="s">
+        <v>167</v>
+      </c>
+      <c r="F6" s="23">
+        <v>522</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>-507</v>
+      </c>
+      <c r="H6">
+        <v>-400</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>-12740.91</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="2"/>
+        <v>-10052</v>
+      </c>
+      <c r="K6">
+        <v>500</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="3"/>
+        <v>50963.64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>140</v>
       </c>
@@ -3041,8 +3372,36 @@
       <c r="C7" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E7" t="s">
+        <v>171</v>
+      </c>
+      <c r="F7" s="23">
+        <v>769</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>-754</v>
+      </c>
+      <c r="H7">
+        <v>-400</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="1"/>
+        <v>-18948.02</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="2"/>
+        <v>-10052</v>
+      </c>
+      <c r="K7">
+        <v>500</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="3"/>
+        <v>75792.08</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>106</v>
       </c>
@@ -3052,8 +3411,36 @@
       <c r="C8" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E8" t="s">
+        <v>176</v>
+      </c>
+      <c r="F8" s="23">
+        <v>1314</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>-1299</v>
+      </c>
+      <c r="H8">
+        <v>-400</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="1"/>
+        <v>-32643.87</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="2"/>
+        <v>-10052</v>
+      </c>
+      <c r="K8">
+        <v>500</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="3"/>
+        <v>130575.48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>107</v>
       </c>
@@ -3064,7 +3451,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>108</v>
       </c>
@@ -3075,18 +3462,18 @@
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B12" s="2"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>84</v>
       </c>
@@ -3103,55 +3490,65 @@
         <v>87</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>103</v>
       </c>
-      <c r="B15" s="22">
+      <c r="B16">
         <v>-1175</v>
       </c>
-      <c r="C15">
+      <c r="C16">
         <v>-400</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D16" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>104</v>
-      </c>
-      <c r="B16" s="22">
-        <f>B15*25.13</f>
-        <v>-29527.75</v>
-      </c>
-      <c r="C16">
-        <f>C15*25.13</f>
-        <v>-10052</v>
-      </c>
-      <c r="D16" t="s">
-        <v>101</v>
-      </c>
-      <c r="E16" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>109</v>
-      </c>
-      <c r="B17" s="22">
-        <v>500</v>
+        <v>104</v>
+      </c>
+      <c r="B17">
+        <f>B16*25.13</f>
+        <v>-29527.75</v>
       </c>
       <c r="C17">
-        <f>ABS(B16)*4</f>
-        <v>118111</v>
+        <f>C16*25.13</f>
+        <v>-10052</v>
       </c>
       <c r="D17" t="s">
         <v>101</v>
       </c>
       <c r="E17" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>109</v>
+      </c>
+      <c r="B18">
+        <v>500</v>
+      </c>
+      <c r="C18">
+        <f>ABS(B17)*4</f>
+        <v>118111</v>
+      </c>
+      <c r="D18" t="s">
+        <v>101</v>
+      </c>
+      <c r="E18" t="s">
         <v>142</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -3163,7 +3560,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FC147DE-C2D1-4559-861B-2B8673B56208}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -3289,4 +3686,308 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5236045A-41A7-AF40-95B6-DBF867B04F6F}">
+  <dimension ref="A1:J10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>3645</v>
+      </c>
+      <c r="F2" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="H2" t="s">
+        <v>155</v>
+      </c>
+      <c r="I2" s="25">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="J2" s="19">
+        <f>$B$10+I2*(1-$B$10)</f>
+        <v>0.28505000000000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C3" t="s">
+        <v>153</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>2817</v>
+      </c>
+      <c r="F3" s="23">
+        <v>894</v>
+      </c>
+      <c r="G3" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="H3" t="s">
+        <v>158</v>
+      </c>
+      <c r="I3" s="25">
+        <v>0</v>
+      </c>
+      <c r="J3" s="19">
+        <f t="shared" ref="J3:J8" si="0">$B$10+I3*(1-$B$10)</f>
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>159</v>
+      </c>
+      <c r="B4" t="s">
+        <v>160</v>
+      </c>
+      <c r="C4" t="s">
+        <v>153</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>3853</v>
+      </c>
+      <c r="F4" s="23">
+        <v>1280</v>
+      </c>
+      <c r="G4" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="H4" t="s">
+        <v>162</v>
+      </c>
+      <c r="I4" s="25">
+        <v>0</v>
+      </c>
+      <c r="J4" s="19">
+        <f t="shared" si="0"/>
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>163</v>
+      </c>
+      <c r="B5" t="s">
+        <v>164</v>
+      </c>
+      <c r="C5" t="s">
+        <v>153</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>3411</v>
+      </c>
+      <c r="F5" s="23" t="s">
+        <v>181</v>
+      </c>
+      <c r="G5" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="H5" t="s">
+        <v>166</v>
+      </c>
+      <c r="I5" s="25">
+        <v>8.8400000000000006E-2</v>
+      </c>
+      <c r="J5" s="19">
+        <f t="shared" si="0"/>
+        <v>0.27983599999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>167</v>
+      </c>
+      <c r="B6" t="s">
+        <v>168</v>
+      </c>
+      <c r="C6" t="s">
+        <v>153</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>1677</v>
+      </c>
+      <c r="F6" s="23" t="s">
+        <v>182</v>
+      </c>
+      <c r="G6" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="H6" t="s">
+        <v>170</v>
+      </c>
+      <c r="I6" s="25">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="J6" s="19">
+        <f t="shared" si="0"/>
+        <v>0.28742000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>171</v>
+      </c>
+      <c r="B7" t="s">
+        <v>172</v>
+      </c>
+      <c r="C7" t="s">
+        <v>173</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>2419</v>
+      </c>
+      <c r="F7" s="23">
+        <v>769</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="H7" t="s">
+        <v>175</v>
+      </c>
+      <c r="I7" s="25">
+        <v>7.8100000000000003E-2</v>
+      </c>
+      <c r="J7" s="19">
+        <f t="shared" si="0"/>
+        <v>0.27169900000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>176</v>
+      </c>
+      <c r="B8" t="s">
+        <v>177</v>
+      </c>
+      <c r="C8" t="s">
+        <v>153</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <v>3990</v>
+      </c>
+      <c r="F8" s="23" t="s">
+        <v>183</v>
+      </c>
+      <c r="G8" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="H8" t="s">
+        <v>179</v>
+      </c>
+      <c r="I8" s="25">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="J8" s="19">
+        <f t="shared" si="0"/>
+        <v>0.24870999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H9" s="18"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>185</v>
+      </c>
+      <c r="B10" s="24">
+        <v>0.21</v>
+      </c>
+      <c r="G10" s="22"/>
+      <c r="H10" s="18"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{E420822C-9CB6-0543-ADF1-EDCFE8D5ABAC}"/>
+    <hyperlink ref="G3" r:id="rId2" display="https://en.wikipedia.org/wiki/Davis%E2%80%93Besse_Nuclear_Power_Station" xr:uid="{9110542E-89D6-2D47-BAB0-04E98B13FBF5}"/>
+    <hyperlink ref="G4" r:id="rId3" xr:uid="{D1783477-78FF-784B-9A1B-672979000EC5}"/>
+    <hyperlink ref="G5" r:id="rId4" xr:uid="{50BD1FBC-1D61-6F40-B26D-85ED74F24A2B}"/>
+    <hyperlink ref="G6" r:id="rId5" xr:uid="{3096E627-E5FC-5A4A-BC59-39F664A94478}"/>
+    <hyperlink ref="G7" r:id="rId6" xr:uid="{A9BD79D7-5527-A44C-B2EE-3F868C0E23D5}"/>
+    <hyperlink ref="G8" r:id="rId7" xr:uid="{9DA2C91F-A18F-F04F-A835-EC8502AD4D48}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Higher lower bound for storage capacity to make dispatch problem feasible
</commit_message>
<xml_diff>
--- a/use_cases/IES_Feb23/data/HERON_data.xlsx
+++ b/use_cases/IES_Feb23/data/HERON_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11009"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrm/FORCE/use_cases/IES_Feb23/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{160E53F7-2C21-874C-BC96-45BE68DCA324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B380733-5988-BD40-8C88-D13629D93DAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17800" windowHeight="22400" activeTab="4" xr2:uid="{3CE7F202-39F9-48AF-B0C7-575379157397}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="29080" windowHeight="20200" activeTab="4" xr2:uid="{3CE7F202-39F9-48AF-B0C7-575379157397}"/>
   </bookViews>
   <sheets>
     <sheet name="MACRS" sheetId="1" r:id="rId1"/>
@@ -789,7 +789,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -813,13 +813,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -2250,10 +2249,10 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="21"/>
+      <c r="B2" s="24"/>
       <c r="C2" t="s">
         <v>4</v>
       </c>
@@ -2421,26 +2420,26 @@
       <c r="B4" s="18"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -2512,15 +2511,15 @@
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -2598,22 +2597,22 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="21" t="s">
+      <c r="A15" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="21"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="21" t="s">
+      <c r="A16" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="B16" s="21"/>
-      <c r="C16" s="21"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
@@ -2627,11 +2626,11 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="21" t="s">
+      <c r="A18" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="B18" s="21"/>
-      <c r="C18" s="21"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
@@ -3131,7 +3130,7 @@
   <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3186,7 +3185,7 @@
       <c r="E2" t="s">
         <v>151</v>
       </c>
-      <c r="F2" s="23">
+      <c r="F2">
         <v>1194</v>
       </c>
       <c r="G2">
@@ -3205,7 +3204,8 @@
         <v>-10052</v>
       </c>
       <c r="K2">
-        <v>500</v>
+        <f>ABS(I2-25.13*H2)*2</f>
+        <v>39152.54</v>
       </c>
       <c r="L2">
         <f>ABS(I2)*4</f>
@@ -3219,7 +3219,7 @@
       <c r="E3" t="s">
         <v>156</v>
       </c>
-      <c r="F3" s="23">
+      <c r="F3">
         <v>894</v>
       </c>
       <c r="G3">
@@ -3238,10 +3238,11 @@
         <v>-10052</v>
       </c>
       <c r="K3">
-        <v>500</v>
+        <f t="shared" ref="K3:K8" si="3">ABS(I3-25.13*H3)*2</f>
+        <v>24074.54</v>
       </c>
       <c r="L3">
-        <f t="shared" ref="L3:L8" si="3">ABS(I3)*4</f>
+        <f t="shared" ref="L3:L8" si="4">ABS(I3)*4</f>
         <v>88357.08</v>
       </c>
     </row>
@@ -3258,7 +3259,7 @@
       <c r="E4" t="s">
         <v>159</v>
       </c>
-      <c r="F4" s="23">
+      <c r="F4">
         <v>1280</v>
       </c>
       <c r="G4">
@@ -3277,10 +3278,11 @@
         <v>-10052</v>
       </c>
       <c r="K4">
-        <v>500</v>
+        <f t="shared" si="3"/>
+        <v>43474.899999999994</v>
       </c>
       <c r="L4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>127157.79999999999</v>
       </c>
     </row>
@@ -3297,7 +3299,7 @@
       <c r="E5" t="s">
         <v>163</v>
       </c>
-      <c r="F5" s="23">
+      <c r="F5">
         <v>1138</v>
       </c>
       <c r="G5">
@@ -3316,10 +3318,11 @@
         <v>-10052</v>
       </c>
       <c r="K5">
-        <v>500</v>
+        <f t="shared" si="3"/>
+        <v>36337.979999999996</v>
       </c>
       <c r="L5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>112883.95999999999</v>
       </c>
     </row>
@@ -3336,7 +3339,7 @@
       <c r="E6" t="s">
         <v>167</v>
       </c>
-      <c r="F6" s="23">
+      <c r="F6">
         <v>522</v>
       </c>
       <c r="G6">
@@ -3355,10 +3358,11 @@
         <v>-10052</v>
       </c>
       <c r="K6">
-        <v>500</v>
+        <f t="shared" si="3"/>
+        <v>5377.82</v>
       </c>
       <c r="L6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>50963.64</v>
       </c>
     </row>
@@ -3375,7 +3379,7 @@
       <c r="E7" t="s">
         <v>171</v>
       </c>
-      <c r="F7" s="23">
+      <c r="F7">
         <v>769</v>
       </c>
       <c r="G7">
@@ -3394,10 +3398,11 @@
         <v>-10052</v>
       </c>
       <c r="K7">
-        <v>500</v>
+        <f t="shared" si="3"/>
+        <v>17792.04</v>
       </c>
       <c r="L7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>75792.08</v>
       </c>
     </row>
@@ -3414,7 +3419,7 @@
       <c r="E8" t="s">
         <v>176</v>
       </c>
-      <c r="F8" s="23">
+      <c r="F8">
         <v>1314</v>
       </c>
       <c r="G8">
@@ -3433,10 +3438,11 @@
         <v>-10052</v>
       </c>
       <c r="K8">
-        <v>500</v>
+        <f t="shared" si="3"/>
+        <v>45183.74</v>
       </c>
       <c r="L8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>130575.48</v>
       </c>
     </row>
@@ -3750,7 +3756,7 @@
       <c r="E2">
         <v>3645</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="F2" t="s">
         <v>180</v>
       </c>
       <c r="G2" s="18" t="s">
@@ -3759,7 +3765,7 @@
       <c r="H2" t="s">
         <v>155</v>
       </c>
-      <c r="I2" s="25">
+      <c r="I2" s="23">
         <v>9.5000000000000001E-2</v>
       </c>
       <c r="J2" s="19">
@@ -3783,7 +3789,7 @@
       <c r="E3">
         <v>2817</v>
       </c>
-      <c r="F3" s="23">
+      <c r="F3">
         <v>894</v>
       </c>
       <c r="G3" s="18" t="s">
@@ -3792,7 +3798,7 @@
       <c r="H3" t="s">
         <v>158</v>
       </c>
-      <c r="I3" s="25">
+      <c r="I3" s="23">
         <v>0</v>
       </c>
       <c r="J3" s="19">
@@ -3816,7 +3822,7 @@
       <c r="E4">
         <v>3853</v>
       </c>
-      <c r="F4" s="23">
+      <c r="F4">
         <v>1280</v>
       </c>
       <c r="G4" s="18" t="s">
@@ -3825,7 +3831,7 @@
       <c r="H4" t="s">
         <v>162</v>
       </c>
-      <c r="I4" s="25">
+      <c r="I4" s="23">
         <v>0</v>
       </c>
       <c r="J4" s="19">
@@ -3849,7 +3855,7 @@
       <c r="E5">
         <v>3411</v>
       </c>
-      <c r="F5" s="23" t="s">
+      <c r="F5" t="s">
         <v>181</v>
       </c>
       <c r="G5" s="18" t="s">
@@ -3858,7 +3864,7 @@
       <c r="H5" t="s">
         <v>166</v>
       </c>
-      <c r="I5" s="25">
+      <c r="I5" s="23">
         <v>8.8400000000000006E-2</v>
       </c>
       <c r="J5" s="19">
@@ -3882,7 +3888,7 @@
       <c r="E6">
         <v>1677</v>
       </c>
-      <c r="F6" s="23" t="s">
+      <c r="F6" t="s">
         <v>182</v>
       </c>
       <c r="G6" s="18" t="s">
@@ -3891,7 +3897,7 @@
       <c r="H6" t="s">
         <v>170</v>
       </c>
-      <c r="I6" s="25">
+      <c r="I6" s="23">
         <v>9.8000000000000004E-2</v>
       </c>
       <c r="J6" s="19">
@@ -3915,7 +3921,7 @@
       <c r="E7">
         <v>2419</v>
       </c>
-      <c r="F7" s="23">
+      <c r="F7">
         <v>769</v>
       </c>
       <c r="G7" s="18" t="s">
@@ -3924,7 +3930,7 @@
       <c r="H7" t="s">
         <v>175</v>
       </c>
-      <c r="I7" s="25">
+      <c r="I7" s="23">
         <v>7.8100000000000003E-2</v>
       </c>
       <c r="J7" s="19">
@@ -3948,7 +3954,7 @@
       <c r="E8">
         <v>3990</v>
       </c>
-      <c r="F8" s="23" t="s">
+      <c r="F8" t="s">
         <v>183</v>
       </c>
       <c r="G8" s="18" t="s">
@@ -3957,7 +3963,7 @@
       <c r="H8" t="s">
         <v>179</v>
       </c>
-      <c r="I8" s="25">
+      <c r="I8" s="23">
         <v>4.9000000000000002E-2</v>
       </c>
       <c r="J8" s="19">
@@ -3972,10 +3978,10 @@
       <c r="A10" t="s">
         <v>185</v>
       </c>
-      <c r="B10" s="24">
+      <c r="B10" s="22">
         <v>0.21</v>
       </c>
-      <c r="G10" s="22"/>
+      <c r="G10" s="21"/>
       <c r="H10" s="18"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update HERON model data
</commit_message>
<xml_diff>
--- a/use_cases/IES_Feb23/data/HERON_data.xlsx
+++ b/use_cases/IES_Feb23/data/HERON_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrm/FORCE/use_cases/IES_Feb23/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B380733-5988-BD40-8C88-D13629D93DAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB96DDC0-F79E-7648-A83A-C086DE2FFA2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="29080" windowHeight="20200" activeTab="4" xr2:uid="{3CE7F202-39F9-48AF-B0C7-575379157397}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="29080" windowHeight="20200" activeTab="3" xr2:uid="{3CE7F202-39F9-48AF-B0C7-575379157397}"/>
   </bookViews>
   <sheets>
     <sheet name="MACRS" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="219">
   <si>
     <t>Source</t>
   </si>
@@ -620,6 +620,84 @@
   </si>
   <si>
     <t>H2 storage Upper (kg-h2)</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>TDCC</t>
+  </si>
+  <si>
+    <t>Total Direct Capital Costs, sum of equipment installed costs</t>
+  </si>
+  <si>
+    <t>$USD (2016)</t>
+  </si>
+  <si>
+    <t>Depreciable Capital Costs</t>
+  </si>
+  <si>
+    <t>Site preparation</t>
+  </si>
+  <si>
+    <t>Eng and design</t>
+  </si>
+  <si>
+    <t>Project contingency</t>
+  </si>
+  <si>
+    <t>Catalyst first fill fee</t>
+  </si>
+  <si>
+    <t>Upfront permitting costs</t>
+  </si>
+  <si>
+    <t>Total depreciable capital costs</t>
+  </si>
+  <si>
+    <t>Non-depreciable Capital Costs</t>
+  </si>
+  <si>
+    <t>Land</t>
+  </si>
+  <si>
+    <t>Total Capital Investment</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>Labor Cost</t>
+  </si>
+  <si>
+    <t>$USD (2016)/year</t>
+  </si>
+  <si>
+    <t>Gen and admin</t>
+  </si>
+  <si>
+    <t>20% LC</t>
+  </si>
+  <si>
+    <t>Property taxes and insurance</t>
+  </si>
+  <si>
+    <t>2% TCI</t>
+  </si>
+  <si>
+    <t>Materials costs for maintenance</t>
+  </si>
+  <si>
+    <t>Total Fixed Operating Costs</t>
+  </si>
+  <si>
+    <t>None Energy material and utilities costs</t>
+  </si>
+  <si>
+    <t>Total Variable Operating Costs (excl. feedstock and elec)</t>
+  </si>
+  <si>
+    <t>Depreciation schedule</t>
   </si>
 </sst>
 </file>
@@ -629,7 +707,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -674,6 +752,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF008000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -688,7 +773,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -782,14 +867,78 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -819,8 +968,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
+    <cellStyle name="Currency" xfId="4" builtinId="4"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1892,15 +2052,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>672042</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>83607</xdr:rowOff>
+      <xdr:colOff>534459</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>42332</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>1333500</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>31751</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2848,42 +3008,88 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D919D22-7A01-ED42-B8B2-84358A3D7717}">
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.6640625" customWidth="1"/>
+    <col min="13" max="13" width="43.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.6640625" customWidth="1"/>
+    <col min="15" max="15" width="18.6640625" customWidth="1"/>
+    <col min="16" max="16" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
       <c r="B2" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M2" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="N2" s="30" t="s">
+        <v>193</v>
+      </c>
+      <c r="O2" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="P2" s="31" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="8" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M3" s="33" t="s">
+        <v>194</v>
+      </c>
+      <c r="N3" s="26" t="s">
+        <v>195</v>
+      </c>
+      <c r="O3" s="27">
+        <v>257800644</v>
+      </c>
+      <c r="P3" s="14" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M4" s="33" t="s">
+        <v>197</v>
+      </c>
+      <c r="N4" s="26" t="s">
+        <v>198</v>
+      </c>
+      <c r="O4" s="27">
+        <v>5156012.88</v>
+      </c>
+      <c r="P4" s="14" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>113</v>
       </c>
@@ -2893,8 +3099,18 @@
       <c r="H5" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M5" s="33"/>
+      <c r="N5" s="26" t="s">
+        <v>199</v>
+      </c>
+      <c r="O5" s="27">
+        <v>25780064.399999999</v>
+      </c>
+      <c r="P5" s="14" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>114</v>
       </c>
@@ -2913,12 +3129,22 @@
       <c r="K6">
         <v>1000</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M6" s="33"/>
+      <c r="N6" s="26" t="s">
+        <v>200</v>
+      </c>
+      <c r="O6" s="27">
+        <v>38670096.600000001</v>
+      </c>
+      <c r="P6" s="14" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>116</v>
       </c>
-      <c r="B7" s="19">
+      <c r="B7">
         <v>1.9E-2</v>
       </c>
       <c r="H7" t="s">
@@ -2933,8 +3159,18 @@
       <c r="K7">
         <v>293926000</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M7" s="33"/>
+      <c r="N7" s="26" t="s">
+        <v>201</v>
+      </c>
+      <c r="O7" s="27">
+        <v>12251143</v>
+      </c>
+      <c r="P7" s="14" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>117</v>
       </c>
@@ -2955,8 +3191,18 @@
         <f>K6/J6</f>
         <v>2.5</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M8" s="33"/>
+      <c r="N8" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="O8" s="27">
+        <v>38670096.600000001</v>
+      </c>
+      <c r="P8" s="14" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>128</v>
       </c>
@@ -2978,8 +3224,18 @@
         <f t="shared" si="0"/>
         <v>0.3979400086720376</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M9" s="33" t="s">
+        <v>203</v>
+      </c>
+      <c r="N9" s="26"/>
+      <c r="O9" s="27">
+        <v>120527413.48</v>
+      </c>
+      <c r="P9" s="14" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H10" t="s">
         <v>133</v>
       </c>
@@ -2995,13 +3251,37 @@
         <f t="shared" si="1"/>
         <v>8.4682380044363352</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M10" s="33" t="s">
+        <v>204</v>
+      </c>
+      <c r="N10" s="26" t="s">
+        <v>205</v>
+      </c>
+      <c r="O10" s="27">
+        <v>550360</v>
+      </c>
+      <c r="P10" s="14" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M11" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="N11" s="26" t="s">
+        <v>206</v>
+      </c>
+      <c r="O11" s="28">
+        <v>378878417.48000002</v>
+      </c>
+      <c r="P11" s="14" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>123</v>
       </c>
@@ -3014,16 +3294,40 @@
       <c r="D12" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M12" s="33" t="s">
+        <v>207</v>
+      </c>
+      <c r="N12" s="26" t="s">
+        <v>208</v>
+      </c>
+      <c r="O12" s="27">
+        <v>9607972</v>
+      </c>
+      <c r="P12" s="14" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>120</v>
       </c>
       <c r="B13" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M13" s="33" t="s">
+        <v>210</v>
+      </c>
+      <c r="N13" s="26" t="s">
+        <v>211</v>
+      </c>
+      <c r="O13" s="27">
+        <v>1921594.4</v>
+      </c>
+      <c r="P13" s="14" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>122</v>
       </c>
@@ -3036,8 +3340,20 @@
       <c r="D14" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M14" s="33" t="s">
+        <v>212</v>
+      </c>
+      <c r="N14" s="26" t="s">
+        <v>213</v>
+      </c>
+      <c r="O14" s="27">
+        <v>7577568.3499999996</v>
+      </c>
+      <c r="P14" s="14" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>130</v>
       </c>
@@ -3048,8 +3364,18 @@
       <c r="C15" s="1" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M15" s="33" t="s">
+        <v>214</v>
+      </c>
+      <c r="N15" s="26"/>
+      <c r="O15" s="27">
+        <v>1049006</v>
+      </c>
+      <c r="P15" s="14" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>85</v>
       </c>
@@ -3057,8 +3383,18 @@
         <v>0.626</v>
       </c>
       <c r="C16" s="1"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="M16" s="33" t="s">
+        <v>215</v>
+      </c>
+      <c r="N16" s="26"/>
+      <c r="O16" s="28">
+        <v>20156140.75</v>
+      </c>
+      <c r="P16" s="14" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>86</v>
       </c>
@@ -3068,16 +3404,50 @@
       <c r="C17" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="M17" s="33" t="s">
+        <v>216</v>
+      </c>
+      <c r="N17" s="26"/>
+      <c r="O17" s="27">
+        <v>7085933</v>
+      </c>
+      <c r="P17" s="14" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="M18" s="33" t="s">
+        <v>217</v>
+      </c>
+      <c r="N18" s="26"/>
+      <c r="O18" s="28">
+        <v>7085933</v>
+      </c>
+      <c r="P18" s="14" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>134</v>
       </c>
       <c r="B19" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="M19" s="34" t="s">
+        <v>218</v>
+      </c>
+      <c r="N19" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="O19" s="29">
+        <v>20</v>
+      </c>
+      <c r="P19" s="17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>120</v>
       </c>
@@ -3085,21 +3455,22 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>130</v>
       </c>
-      <c r="B21" s="20" t="e">
-        <f>POWER(1+B7,4)*#REF!</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B21" s="20">
+        <f>POWER(1+B7,4)*O18</f>
+        <v>7640007.3719816608</v>
+      </c>
+      <c r="O21" s="25"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>120</v>
       </c>
@@ -3107,13 +3478,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>130</v>
       </c>
-      <c r="B25" s="20" t="e">
-        <f>POWER(1+B7,4)*#REF!</f>
-        <v>#REF!</v>
+      <c r="B25" s="20">
+        <f>POWER(1+B7,4)*O16</f>
+        <v>21732221.278510533</v>
       </c>
       <c r="C25" t="s">
         <v>136</v>
@@ -3129,7 +3500,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9241F20-95C4-42A2-B03A-23B9DD4DBFA3}">
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Sort sweep golded files
</commit_message>
<xml_diff>
--- a/use_cases/IES_Feb23/data/HERON_data.xlsx
+++ b/use_cases/IES_Feb23/data/HERON_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrm/FORCE/use_cases/IES_Feb23/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FBB5A99-0DF9-5D48-AE40-071EC3E00078}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DEF6994-BF94-D64B-ADBF-DC2D3CE21483}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11420" yWindow="500" windowWidth="19300" windowHeight="17000" activeTab="4" xr2:uid="{3CE7F202-39F9-48AF-B0C7-575379157397}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="30720" windowHeight="17000" activeTab="4" xr2:uid="{3CE7F202-39F9-48AF-B0C7-575379157397}"/>
   </bookViews>
   <sheets>
     <sheet name="MACRS" sheetId="1" r:id="rId1"/>
@@ -3492,8 +3492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9241F20-95C4-42A2-B03A-23B9DD4DBFA3}">
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3554,15 +3554,15 @@
         <v>1194</v>
       </c>
       <c r="G2">
-        <f>-F2+15</f>
-        <v>-1179</v>
+        <f>-F2+14.9</f>
+        <v>-1179.0999999999999</v>
       </c>
       <c r="H2">
         <v>-100</v>
       </c>
       <c r="I2">
         <f>G2*25.13</f>
-        <v>-29628.27</v>
+        <v>-29630.782999999996</v>
       </c>
       <c r="J2">
         <f>H2*25.13</f>
@@ -3570,11 +3570,11 @@
       </c>
       <c r="K2">
         <f>ABS(I2-25.13*H2)*2</f>
-        <v>54230.54</v>
+        <v>54235.565999999992</v>
       </c>
       <c r="L2">
         <f>ABS(I2)*4</f>
-        <v>118513.08</v>
+        <v>118523.13199999998</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -3588,15 +3588,15 @@
         <v>894</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G8" si="0">-F3+15</f>
-        <v>-879</v>
+        <f t="shared" ref="G3:G8" si="0">-F3+14.9</f>
+        <v>-879.1</v>
       </c>
       <c r="H3">
         <v>-100</v>
       </c>
       <c r="I3">
         <f t="shared" ref="I3:I8" si="1">G3*25.13</f>
-        <v>-22089.27</v>
+        <v>-22091.782999999999</v>
       </c>
       <c r="J3">
         <f t="shared" ref="J3:J8" si="2">H3*25.13</f>
@@ -3604,11 +3604,11 @@
       </c>
       <c r="K3">
         <f t="shared" ref="K3:K8" si="3">ABS(I3-25.13*H3)*2</f>
-        <v>39152.54</v>
+        <v>39157.565999999999</v>
       </c>
       <c r="L3">
         <f t="shared" ref="L3:L8" si="4">ABS(I3)*4</f>
-        <v>88357.08</v>
+        <v>88367.131999999998</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -3629,14 +3629,14 @@
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
-        <v>-1265</v>
+        <v>-1265.0999999999999</v>
       </c>
       <c r="H4">
         <v>-100</v>
       </c>
       <c r="I4">
         <f t="shared" si="1"/>
-        <v>-31789.449999999997</v>
+        <v>-31791.962999999996</v>
       </c>
       <c r="J4">
         <f t="shared" si="2"/>
@@ -3644,11 +3644,11 @@
       </c>
       <c r="K4">
         <f t="shared" si="3"/>
-        <v>58552.899999999994</v>
+        <v>58557.925999999992</v>
       </c>
       <c r="L4">
         <f t="shared" si="4"/>
-        <v>127157.79999999999</v>
+        <v>127167.85199999998</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -3669,14 +3669,14 @@
       </c>
       <c r="G5">
         <f t="shared" si="0"/>
-        <v>-1123</v>
+        <v>-1123.0999999999999</v>
       </c>
       <c r="H5">
         <v>-100</v>
       </c>
       <c r="I5">
         <f t="shared" si="1"/>
-        <v>-28220.989999999998</v>
+        <v>-28223.502999999997</v>
       </c>
       <c r="J5">
         <f t="shared" si="2"/>
@@ -3684,11 +3684,11 @@
       </c>
       <c r="K5">
         <f t="shared" si="3"/>
-        <v>51415.979999999996</v>
+        <v>51421.005999999994</v>
       </c>
       <c r="L5">
         <f t="shared" si="4"/>
-        <v>112883.95999999999</v>
+        <v>112894.01199999999</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -3709,14 +3709,14 @@
       </c>
       <c r="G6">
         <f t="shared" si="0"/>
-        <v>-507</v>
+        <v>-507.1</v>
       </c>
       <c r="H6">
         <v>-100</v>
       </c>
       <c r="I6">
         <f t="shared" si="1"/>
-        <v>-12740.91</v>
+        <v>-12743.423000000001</v>
       </c>
       <c r="J6">
         <f t="shared" si="2"/>
@@ -3724,11 +3724,11 @@
       </c>
       <c r="K6">
         <f t="shared" si="3"/>
-        <v>20455.82</v>
+        <v>20460.846000000001</v>
       </c>
       <c r="L6">
         <f t="shared" si="4"/>
-        <v>50963.64</v>
+        <v>50973.692000000003</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -3749,14 +3749,14 @@
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
-        <v>-754</v>
+        <v>-754.1</v>
       </c>
       <c r="H7">
         <v>-100</v>
       </c>
       <c r="I7">
         <f t="shared" si="1"/>
-        <v>-18948.02</v>
+        <v>-18950.532999999999</v>
       </c>
       <c r="J7">
         <f t="shared" si="2"/>
@@ -3764,11 +3764,11 @@
       </c>
       <c r="K7">
         <f t="shared" si="3"/>
-        <v>32870.04</v>
+        <v>32875.065999999999</v>
       </c>
       <c r="L7">
         <f t="shared" si="4"/>
-        <v>75792.08</v>
+        <v>75802.131999999998</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -3789,14 +3789,14 @@
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
-        <v>-1299</v>
+        <v>-1299.0999999999999</v>
       </c>
       <c r="H8">
         <v>-100</v>
       </c>
       <c r="I8">
         <f t="shared" si="1"/>
-        <v>-32643.87</v>
+        <v>-32646.382999999998</v>
       </c>
       <c r="J8">
         <f t="shared" si="2"/>
@@ -3804,11 +3804,11 @@
       </c>
       <c r="K8">
         <f t="shared" si="3"/>
-        <v>60261.74</v>
+        <v>60266.765999999996</v>
       </c>
       <c r="L8">
         <f t="shared" si="4"/>
-        <v>130575.48</v>
+        <v>130585.53199999999</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">

</xml_diff>